<commit_message>
Fix column headers for CompanySyncModel XLSX file
</commit_message>
<xml_diff>
--- a/Example Sync Files/company.xlsx
+++ b/Example Sync Files/company.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheodoreSpence\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\lockstep-sdk-examples\Example Sync Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E759A46D-B268-41E4-83C7-81FAE22BE020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAD830A-849B-4654-BD92-A1FD6A46DBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,24 +43,6 @@
     <t>address1</t>
   </si>
   <si>
-    <t>corpCity</t>
-  </si>
-  <si>
-    <t>corpState</t>
-  </si>
-  <si>
-    <t>corpPostalCode</t>
-  </si>
-  <si>
-    <t>corpCountry</t>
-  </si>
-  <si>
-    <t>corpPhone</t>
-  </si>
-  <si>
-    <t>corpFax</t>
-  </si>
-  <si>
     <t>created</t>
   </si>
   <si>
@@ -602,6 +584,24 @@
   </si>
   <si>
     <t>346E48B3-44A2-45DB-B6E8-8A18517B514E</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>stateRegion</t>
+  </si>
+  <si>
+    <t>postalCode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>faxNumber</t>
   </si>
 </sst>
 </file>
@@ -673,6 +673,23 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -701,23 +718,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -732,7 +732,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2074B1BA-5F6B-49D1-8796-B148D3341D0A}" name="Table1" displayName="Table1" ref="A1:T23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2074B1BA-5F6B-49D1-8796-B148D3341D0A}" name="Table1" displayName="Table1" ref="A1:T23" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:T23" xr:uid="{2074B1BA-5F6B-49D1-8796-B148D3341D0A}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{EF49A329-C0CB-471C-9323-52B5F5FDB3AD}" name="companyName"/>
@@ -742,14 +742,14 @@
     <tableColumn id="5" xr3:uid="{D5B4F745-5AA1-4AEC-A89D-05ABAED89AF7}" name="isActive"/>
     <tableColumn id="6" xr3:uid="{51DDCCEE-C318-489E-A80B-0EFE89E02295}" name="defaultCurrencyCode"/>
     <tableColumn id="7" xr3:uid="{8C3D2104-6745-46E8-9732-CDC4BABA9286}" name="address1"/>
-    <tableColumn id="8" xr3:uid="{E43D89E1-B36B-4003-8186-0929850294F1}" name="corpCity"/>
-    <tableColumn id="9" xr3:uid="{AD729E57-00DF-4469-8E3A-9803AEAE07C0}" name="corpState"/>
-    <tableColumn id="10" xr3:uid="{A0915248-2767-484A-A2F7-43AE7588E000}" name="corpPostalCode"/>
-    <tableColumn id="11" xr3:uid="{D21E2E1F-0789-47E9-BEE7-03C5093D2F07}" name="corpCountry"/>
-    <tableColumn id="12" xr3:uid="{3D0C7729-87B8-48AF-80D9-05DE44B65A13}" name="corpPhone"/>
-    <tableColumn id="13" xr3:uid="{288E0CA7-D372-421E-BC0D-5C08B733E187}" name="corpFax"/>
+    <tableColumn id="8" xr3:uid="{E43D89E1-B36B-4003-8186-0929850294F1}" name="city"/>
+    <tableColumn id="9" xr3:uid="{AD729E57-00DF-4469-8E3A-9803AEAE07C0}" name="stateRegion"/>
+    <tableColumn id="10" xr3:uid="{A0915248-2767-484A-A2F7-43AE7588E000}" name="postalCode"/>
+    <tableColumn id="11" xr3:uid="{D21E2E1F-0789-47E9-BEE7-03C5093D2F07}" name="country"/>
+    <tableColumn id="12" xr3:uid="{3D0C7729-87B8-48AF-80D9-05DE44B65A13}" name="phoneNumber"/>
+    <tableColumn id="13" xr3:uid="{288E0CA7-D372-421E-BC0D-5C08B733E187}" name="faxNumber"/>
     <tableColumn id="14" xr3:uid="{97379B4D-8597-4F13-B3BF-00E9FAA960A7}" name="created"/>
-    <tableColumn id="15" xr3:uid="{9A223682-4862-48C6-8229-A4F6DA50B8CE}" name="modified" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{9A223682-4862-48C6-8229-A4F6DA50B8CE}" name="modified" dataDxfId="0"/>
     <tableColumn id="16" xr3:uid="{CD8322A5-A580-455E-A4A5-6AC8ABE6EB91}" name="taxId"/>
     <tableColumn id="17" xr3:uid="{3085C676-FE78-49E7-81D7-8D9683DD25B6}" name="apEmailAddress"/>
     <tableColumn id="18" xr3:uid="{AFD4649F-60F6-4C5D-B97C-7D6DFB3040C3}" name="arEmailAddress"/>
@@ -1083,8 +1083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,78 +1133,78 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="J2">
         <v>67410</v>
       </c>
       <c r="K2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L2">
         <v>4566882411</v>
@@ -1213,60 +1213,60 @@
         <v>4566882424</v>
       </c>
       <c r="N2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O2" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="R2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="S2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J3">
         <v>19440</v>
       </c>
       <c r="K3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L3">
         <v>1458713524</v>
@@ -1275,60 +1275,60 @@
         <v>1458713530</v>
       </c>
       <c r="N3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O3" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="R3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="S3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J4">
         <v>37211</v>
       </c>
       <c r="K4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L4">
         <v>1379856821</v>
@@ -1337,60 +1337,60 @@
         <v>1379856831</v>
       </c>
       <c r="N4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O4" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P4" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="R4" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="S4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T4" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J5">
         <v>60201</v>
       </c>
       <c r="K5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L5">
         <v>6409751403</v>
@@ -1399,60 +1399,60 @@
         <v>6409751414</v>
       </c>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O5" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P5" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="R5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="S5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T5" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E6" t="b">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J6">
         <v>7050</v>
       </c>
       <c r="K6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L6">
         <v>7697073172</v>
@@ -1461,60 +1461,60 @@
         <v>7697073173</v>
       </c>
       <c r="N6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O6" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P6" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="R6" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="S6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
       </c>
       <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
         <v>67</v>
       </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J7">
         <v>96720</v>
       </c>
       <c r="K7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L7">
         <v>7865822984</v>
@@ -1523,60 +1523,60 @@
         <v>7865823002</v>
       </c>
       <c r="N7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O7" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P7" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q7" t="s">
         <v>128</v>
       </c>
-      <c r="Q7" t="s">
-        <v>134</v>
-      </c>
       <c r="R7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="S7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T7" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="J8">
         <v>63104</v>
       </c>
       <c r="K8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L8">
         <v>5989688246</v>
@@ -1585,60 +1585,60 @@
         <v>5989688251</v>
       </c>
       <c r="N8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O8" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="R8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="S8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T8" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E9" t="b">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="I9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J9">
         <v>1602</v>
       </c>
       <c r="K9" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L9">
         <v>9588447939</v>
@@ -1647,60 +1647,60 @@
         <v>9588447948</v>
       </c>
       <c r="N9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O9" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P9" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="R9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="S9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E10" t="b">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H10" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J10">
         <v>92647</v>
       </c>
       <c r="K10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L10">
         <v>1657233277</v>
@@ -1709,60 +1709,60 @@
         <v>1657233280</v>
       </c>
       <c r="N10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O10" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="R10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="S10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T10" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E11" t="b">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="I11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J11">
         <v>68124</v>
       </c>
       <c r="K11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L11">
         <v>5423492252</v>
@@ -1771,60 +1771,60 @@
         <v>5423492257</v>
       </c>
       <c r="N11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O11" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P11" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q11" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="R11" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="S11" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T11" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E12" t="b">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="J12">
         <v>90016</v>
       </c>
       <c r="K12" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L12">
         <v>2521367145</v>
@@ -1833,60 +1833,60 @@
         <v>2521367157</v>
       </c>
       <c r="N12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O12" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P12" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q12" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="R12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="S12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T12" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J13">
         <v>75149</v>
       </c>
       <c r="K13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L13">
         <v>3513963532</v>
@@ -1895,54 +1895,54 @@
         <v>3513963545</v>
       </c>
       <c r="N13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="O13" s="1">
         <v>44509.503060763891</v>
       </c>
       <c r="P13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q13" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="R13" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E14" t="b">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J14">
         <v>77301</v>
       </c>
       <c r="K14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L14">
         <v>4192883772</v>
@@ -1951,60 +1951,60 @@
         <v>4192883775</v>
       </c>
       <c r="N14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O14" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P14" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="R14" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="S14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T14" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E15" t="b">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I15" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J15">
         <v>22003</v>
       </c>
       <c r="K15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L15">
         <v>4714394218</v>
@@ -2013,60 +2013,60 @@
         <v>4714394236</v>
       </c>
       <c r="N15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O15" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P15" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q15" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="R15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="S15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T15" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="J16">
         <v>7104</v>
       </c>
       <c r="K16" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L16">
         <v>5405715371</v>
@@ -2075,60 +2075,60 @@
         <v>5405715384</v>
       </c>
       <c r="N16" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O16" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q16" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="R16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="S16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T16" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E17" t="b">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H17" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="I17" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J17">
         <v>19103</v>
       </c>
       <c r="K17" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L17">
         <v>4069652125</v>
@@ -2137,60 +2137,60 @@
         <v>4069652139</v>
       </c>
       <c r="N17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O17" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P17" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q17" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="R17" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="S17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T17" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
-        <v>64</v>
-      </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="J18">
         <v>48933</v>
       </c>
       <c r="K18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L18">
         <v>6023923538</v>
@@ -2199,60 +2199,60 @@
         <v>6023923550</v>
       </c>
       <c r="N18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O18" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="R18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="S18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T18" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="I19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J19">
         <v>78664</v>
       </c>
       <c r="K19" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L19">
         <v>9672192969</v>
@@ -2261,60 +2261,60 @@
         <v>9672192980</v>
       </c>
       <c r="N19" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O19" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P19" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q19" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="R19" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T19" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
       </c>
       <c r="E20" t="b">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J20">
         <v>78753</v>
       </c>
       <c r="K20" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L20">
         <v>6835425950</v>
@@ -2323,60 +2323,60 @@
         <v>6835425961</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O20" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P20" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q20" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="R20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="S20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T20" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H21" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" t="s">
         <v>109</v>
-      </c>
-      <c r="I21" t="s">
-        <v>115</v>
       </c>
       <c r="J21">
         <v>8876</v>
       </c>
       <c r="K21" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L21">
         <v>9143548971</v>
@@ -2385,60 +2385,60 @@
         <v>9143548981</v>
       </c>
       <c r="N21" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O21" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P21" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q21" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="R21" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="S21" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T21" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E22" t="b">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I22" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="J22">
         <v>77301</v>
       </c>
       <c r="K22" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L22">
         <v>7733813248</v>
@@ -2447,60 +2447,60 @@
         <v>7733813256</v>
       </c>
       <c r="N22" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O22" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P22" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q22" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="R22" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="S22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T22" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G23" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J23">
         <v>11101</v>
       </c>
       <c r="K23" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L23">
         <v>7175731387</v>
@@ -2509,25 +2509,25 @@
         <v>7175731394</v>
       </c>
       <c r="N23" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="O23" s="1">
         <v>44509.50306087963</v>
       </c>
       <c r="P23" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="Q23" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="R23" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="S23" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="T23" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>